<commit_message>
Created Radioactive Disposal Log
Created a radioactive disposal log, which will be populated with the ligand summary data (3H-Ligand, uCi used, and the 80% 20% for sink disposal and dry waste respectively)

Also updated the binding printout sheet to include the uCi used on the day, for instances when the uCi/uL ratio is not equal to 1
</commit_message>
<xml_diff>
--- a/Python_Scripts/Daily_Radioactivity/data_files/Binding_Printout_Template.xlsx
+++ b/Python_Scripts/Daily_Radioactivity/data_files/Binding_Printout_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kealbert\Documents\Python Scripts\Trying stuff\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D420B02E-F06B-48D2-B061-7B5518826483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87101873-7072-4997-A4BF-274619F33532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,9 +79,6 @@
     <t>P/S</t>
   </si>
   <si>
-    <t>Pellets:</t>
-  </si>
-  <si>
     <t>Ligand Vol (µL)</t>
   </si>
   <si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t># of Pellets</t>
+  </si>
+  <si>
+    <t>Ligand (µCi)</t>
   </si>
 </sst>
 </file>
@@ -144,7 +144,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -259,24 +259,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -320,11 +350,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -346,6 +385,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1108,7 +1156,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,529 +1175,529 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="25"/>
     </row>
     <row r="2" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25" t="s">
+      <c r="F2" s="26"/>
+      <c r="G2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="27"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="29"/>
     </row>
     <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="34"/>
+      <c r="J3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="31"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="14"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="14"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="14"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="14"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="14"/>
+    </row>
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="22" t="s">
+      <c r="E13" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="17"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="17"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="17"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="17"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="17"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="17"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="17"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="17"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="17"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="34" t="s">
+      <c r="F13" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="16"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="17"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="17"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="14"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="17"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="14"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="17"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="14"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="17"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="14"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="17"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="14"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="17"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="14"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="17"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="14"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="17"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="14"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="17"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="14"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="17"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="14"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="17"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="14"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="17"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="14"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="17"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="14"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="17"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="14"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="17"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="14"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="17"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="14"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="18"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="15"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
     </row>
     <row r="33" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="23">
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="H13:H14"/>
@@ -1663,7 +1711,6 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:M2"/>
     <mergeCell ref="A4:A12"/>
-    <mergeCell ref="F4:F12"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>

</xml_diff>